<commit_message>
Update Lista de Tareas final.xlsx
</commit_message>
<xml_diff>
--- a/Lista de Tareas final.xlsx
+++ b/Lista de Tareas final.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21311"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\MULTIMEDIA\Repositorios\proyecto-multimedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9C13FE0-5FDE-4D48-B9F4-218A6D527BC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -191,8 +190,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1149,31 +1148,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="84" zoomScaleNormal="84" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="2" customWidth="1"/>
     <col min="6" max="7" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2"/>
-    <col min="9" max="9" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="2"/>
-    <col min="12" max="12" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="2"/>
+    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.88671875" style="2"/>
+    <col min="12" max="12" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="42" t="s">
         <v>5</v>
       </c>
@@ -1207,7 +1206,7 @@
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="43"/>
       <c r="C4" s="1">
         <f>1+C3</f>
@@ -1222,7 +1221,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="2:7" ht="15">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="44"/>
       <c r="C5" s="10">
         <f t="shared" ref="C5:C27" si="0">1+C4</f>
@@ -1237,7 +1236,7 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="2:7" ht="15">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="45"/>
       <c r="C6" s="51">
         <f>1+C5</f>
@@ -1254,7 +1253,7 @@
       </c>
       <c r="G6" s="13"/>
     </row>
-    <row r="7" spans="2:7" ht="15">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="46"/>
       <c r="C7" s="52"/>
       <c r="D7" s="49"/>
@@ -1266,7 +1265,7 @@
       </c>
       <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="2:7" ht="15">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="46"/>
       <c r="C8" s="52"/>
       <c r="D8" s="49"/>
@@ -1278,7 +1277,7 @@
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="2:7" ht="15">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="46"/>
       <c r="C9" s="52"/>
       <c r="D9" s="49"/>
@@ -1290,7 +1289,7 @@
       </c>
       <c r="G9" s="13"/>
     </row>
-    <row r="10" spans="2:7" ht="15">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="46"/>
       <c r="C10" s="53"/>
       <c r="D10" s="50"/>
@@ -1302,7 +1301,7 @@
       </c>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="2:7" ht="15">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="46"/>
       <c r="C11" s="1">
         <f>1+4</f>
@@ -1317,7 +1316,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="2:7" ht="15">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="46"/>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
@@ -1332,7 +1331,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="2:7" ht="15">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="46"/>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
@@ -1347,7 +1346,7 @@
       </c>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="2:7" ht="15">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="46"/>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
@@ -1362,7 +1361,7 @@
       </c>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="2:7" ht="15">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="46"/>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
@@ -1377,7 +1376,7 @@
       </c>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="2:7" ht="15">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="46"/>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
@@ -1392,7 +1391,7 @@
       </c>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="2:16" ht="15">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="46"/>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
@@ -1407,7 +1406,7 @@
       </c>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="2:16" ht="15">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="46"/>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
@@ -1422,7 +1421,7 @@
       </c>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="2:16" ht="15">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="46"/>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
@@ -1437,7 +1436,7 @@
       </c>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="2:16" ht="15">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="46"/>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
@@ -1452,7 +1451,7 @@
       </c>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="2:16" ht="15">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="47"/>
       <c r="C21" s="51">
         <f>1+C20</f>
@@ -1469,7 +1468,7 @@
       </c>
       <c r="G21" s="41"/>
     </row>
-    <row r="22" spans="2:16" ht="14.45" customHeight="1">
+    <row r="22" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="45" t="s">
         <v>27</v>
       </c>
@@ -1483,7 +1482,7 @@
       </c>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="2:16" ht="14.45" customHeight="1">
+    <row r="23" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="46"/>
       <c r="C23" s="1">
         <f>1+C21</f>
@@ -1498,7 +1497,7 @@
       </c>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="2:16">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="46"/>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
@@ -1513,7 +1512,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="2:16">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="46"/>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
@@ -1528,7 +1527,7 @@
       </c>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="2:16">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="46"/>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
@@ -1543,7 +1542,7 @@
       </c>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="2:16">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="46"/>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
@@ -1558,7 +1557,7 @@
       </c>
       <c r="G27" s="19"/>
     </row>
-    <row r="28" spans="2:16">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="46"/>
       <c r="C28" s="1">
         <f>1+C27</f>
@@ -1592,7 +1591,7 @@
       </c>
       <c r="P28" s="27"/>
     </row>
-    <row r="29" spans="2:16">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="46"/>
       <c r="C29" s="1">
         <f t="shared" ref="C29:C31" si="1">1+C28</f>
@@ -1615,7 +1614,7 @@
       <c r="O29" s="27"/>
       <c r="P29" s="27"/>
     </row>
-    <row r="30" spans="2:16">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="46"/>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
@@ -1636,7 +1635,7 @@
       <c r="O30" s="27"/>
       <c r="P30" s="27"/>
     </row>
-    <row r="31" spans="2:16" ht="15" thickBot="1">
+    <row r="31" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="47"/>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
@@ -1660,7 +1659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:16">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F32" s="4">
         <f>SUM(F3:F31)</f>
         <v>8</v>
@@ -1675,38 +1674,38 @@
         <v>43528</v>
       </c>
     </row>
-    <row r="33" spans="5:7">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
       <c r="G33" s="5">
         <f>F32/(MAX(C3:C31))</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="34" spans="5:7">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E34" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="5:7">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="5:7">
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="5:7">
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="5:7">
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E38" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="5:7">
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E39" s="2" t="s">
         <v>52</v>
       </c>

</xml_diff>